<commit_message>
O 2+ had 1% uncertainties instead of 10%, O5 uncertainties didn't include 11% syst unc
</commit_message>
<xml_diff>
--- a/csdata/O/SI/O0+.xlsx
+++ b/csdata/O/SI/O0+.xlsx
@@ -1,17 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmondeel/Documents/CfA/Chandra/CHANDRA-Rates/csdata/O/SI/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3010F30B-F62B-8D4F-8C01-7DE2EDD268E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15140" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Energy (eV)</t>
   </si>
@@ -30,33 +52,41 @@
   <si>
     <t>Thompson et al 1995 J Phys B Single and double ionization of atomic oxygen by electron impact</t>
   </si>
+  <si>
+    <t>Unc at peak</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -65,54 +95,56 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -302,20 +334,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F1:F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -331,8 +368,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>14.1</v>
       </c>
@@ -340,16 +380,20 @@
         <v>0.24</v>
       </c>
       <c r="C2" s="2">
-        <v>0.0195509590557599</v>
+        <v>1.95509590557599E-2</v>
       </c>
       <c r="D2" s="5">
-        <v>-17.0</v>
+        <v>-17</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="F2">
+        <f>_xlfn.XLOOKUP(MAX(B:B),B:B,C:C)/MAX(B:B)</f>
+        <v>7.5170538580748486E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>14.3</v>
       </c>
@@ -357,12 +401,12 @@
         <v>0.34</v>
       </c>
       <c r="C3" s="2">
-        <v>0.02581549922042958</v>
+        <v>2.581549922042958E-2</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>14.5</v>
       </c>
@@ -370,12 +414,12 @@
         <v>0.47</v>
       </c>
       <c r="C4" s="2">
-        <v>0.03850207786600614</v>
+        <v>3.8502077866006137E-2</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>14.7</v>
       </c>
@@ -383,487 +427,487 @@
         <v>0.41</v>
       </c>
       <c r="C5" s="2">
-        <v>0.034981280708401744</v>
+        <v>3.4981280708401744E-2</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8">
         <v>0.53</v>
       </c>
-      <c r="C6" s="9">
-        <v>0.042147479165425786</v>
+      <c r="C6" s="6">
+        <v>4.2147479165425786E-2</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>15.3</v>
       </c>
       <c r="B7" s="8">
         <v>0.69</v>
       </c>
-      <c r="C7" s="9">
-        <v>0.05685850859809814</v>
+      <c r="C7" s="6">
+        <v>5.6858508598098143E-2</v>
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="7">
         <v>15.7</v>
       </c>
       <c r="B8" s="8">
         <v>0.75</v>
       </c>
-      <c r="C8" s="9">
-        <v>0.06046693311223913</v>
+      <c r="C8" s="6">
+        <v>6.0466933112239128E-2</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="B9" s="8">
         <v>0.99</v>
       </c>
-      <c r="C9" s="9">
-        <v>0.08001556098659811</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9" s="6">
+        <v>8.0015560986598108E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="B10" s="8">
-        <v>1.1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0.09180958555619344</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C10" s="6">
+        <v>9.1809585556193438E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>17.8</v>
       </c>
       <c r="B11" s="8">
         <v>1.52</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>0.12215138149034582</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="7">
         <v>19.2</v>
       </c>
       <c r="B12" s="8">
         <v>2.11</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="6">
         <v>0.16797407538069678</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>21.6</v>
       </c>
       <c r="B13" s="8">
         <v>3.61</v>
       </c>
-      <c r="C13" s="9">
-        <v>0.279745044638864</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="C13" s="6">
+        <v>0.27974504463886402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="7">
         <v>23.2</v>
       </c>
       <c r="B14" s="8">
-        <v>4.36</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0.3445969239560911</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.34459692395609109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>29.2</v>
       </c>
       <c r="B15" s="8">
         <v>6.27</v>
       </c>
-      <c r="C15" s="9">
-        <v>0.486552371281859</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="C15" s="6">
+        <v>0.48655237128185902</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="7">
         <v>31.2</v>
       </c>
       <c r="B16" s="8">
         <v>7.12</v>
       </c>
-      <c r="C16" s="9">
-        <v>0.5531749813576171</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="C16" s="6">
+        <v>0.55317498135761711</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
         <v>35.5</v>
       </c>
       <c r="B17" s="8">
         <v>7.61</v>
       </c>
-      <c r="C17" s="9">
-        <v>0.5927641099121977</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="C17" s="6">
+        <v>0.59276410991219775</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="7">
         <v>40.5</v>
       </c>
       <c r="B18" s="8">
         <v>10.1</v>
       </c>
-      <c r="C18" s="9">
-        <v>0.7680162758692032</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="C18" s="6">
+        <v>0.76801627586920318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="7">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B19" s="8">
         <v>11.8</v>
       </c>
-      <c r="C19" s="9">
-        <v>0.8787923531756522</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="C19" s="6">
+        <v>0.87879235317565219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="7">
-        <v>50.0</v>
-      </c>
-      <c r="B20" s="9">
+        <v>50</v>
+      </c>
+      <c r="B20" s="6">
         <v>12.2</v>
       </c>
-      <c r="C20" s="9">
-        <v>0.9430355242513402</v>
-      </c>
-    </row>
-    <row r="21">
+      <c r="C20" s="6">
+        <v>0.94303552425134018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7">
-        <v>56.0</v>
-      </c>
-      <c r="B21" s="9">
+        <v>56</v>
+      </c>
+      <c r="B21" s="6">
         <v>12.4</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="6">
         <v>0.9557321800588281</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="7">
-        <v>63.0</v>
-      </c>
-      <c r="B22" s="9">
+        <v>63</v>
+      </c>
+      <c r="B22" s="6">
         <v>12.5</v>
       </c>
-      <c r="C22" s="9">
-        <v>0.962094070244693</v>
-      </c>
-    </row>
-    <row r="23">
+      <c r="C22" s="6">
+        <v>0.96209407024469296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="7">
-        <v>71.0</v>
-      </c>
-      <c r="B23" s="9">
-        <v>13.0</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0.9940321926376431</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>71</v>
+      </c>
+      <c r="B23" s="6">
+        <v>13</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.99403219263764309</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="7">
-        <v>80.0</v>
-      </c>
-      <c r="B24" s="9">
+        <v>80</v>
+      </c>
+      <c r="B24" s="6">
         <v>13.1</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="6">
         <v>1.000444401253763</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="9">
-        <v>90.0</v>
-      </c>
-      <c r="B25" s="9">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6">
+        <v>90</v>
+      </c>
+      <c r="B25" s="6">
         <v>14.4</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="6">
         <v>1.0844648449811551</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="9">
-        <v>97.0</v>
-      </c>
-      <c r="B26" s="9">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6">
+        <v>97</v>
+      </c>
+      <c r="B26" s="6">
         <v>14.6</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="6">
         <v>1.0974898632789278</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="9">
-        <v>112.0</v>
-      </c>
-      <c r="B27" s="9">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="6">
+        <v>112</v>
+      </c>
+      <c r="B27" s="6">
         <v>14.5</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="6">
         <v>1.0909743351701726</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="9">
-        <v>126.0</v>
-      </c>
-      <c r="B28" s="9">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="6">
+        <v>126</v>
+      </c>
+      <c r="B28" s="6">
         <v>14.5</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="6">
         <v>1.0909743351701726</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="9">
-        <v>147.0</v>
-      </c>
-      <c r="B29" s="9">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6">
+        <v>147</v>
+      </c>
+      <c r="B29" s="6">
         <v>14.3</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="6">
         <v>1.0779615020955062</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="9">
-        <v>165.0</v>
-      </c>
-      <c r="B30" s="9">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6">
+        <v>165</v>
+      </c>
+      <c r="B30" s="6">
         <v>13.7</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="6">
         <v>1.0390769942598095</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="9">
-        <v>190.0</v>
-      </c>
-      <c r="B31" s="9">
-        <v>13.0</v>
-      </c>
-      <c r="C31" s="9">
-        <v>0.9940321926376431</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="9">
-        <v>219.0</v>
-      </c>
-      <c r="B32" s="9">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="6">
+        <v>190</v>
+      </c>
+      <c r="B31" s="6">
+        <v>13</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.99403219263764309</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="6">
+        <v>219</v>
+      </c>
+      <c r="B32" s="6">
         <v>11.9</v>
       </c>
-      <c r="C32" s="9">
-        <v>0.8853750617676105</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="9">
-        <v>252.0</v>
-      </c>
-      <c r="B33" s="9">
+      <c r="C32" s="6">
+        <v>0.88537506176761049</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="6">
+        <v>252</v>
+      </c>
+      <c r="B33" s="6">
         <v>12.2</v>
       </c>
-      <c r="C33" s="9">
-        <v>0.9051607592024744</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="9">
-        <v>297.0</v>
-      </c>
-      <c r="B34" s="9">
+      <c r="C33" s="6">
+        <v>0.90516075920247441</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="6">
+        <v>297</v>
+      </c>
+      <c r="B34" s="6">
         <v>9.9</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="6">
         <v>0.7551483298001791</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="9">
-        <v>342.0</v>
-      </c>
-      <c r="B35" s="9">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="6">
+        <v>342</v>
+      </c>
+      <c r="B35" s="6">
         <v>9.5</v>
       </c>
-      <c r="C35" s="9">
-        <v>0.7295375247374188</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="9">
-        <v>393.0</v>
-      </c>
-      <c r="B36" s="9">
-        <v>8.8</v>
-      </c>
-      <c r="C36" s="9">
-        <v>0.6851685923916829</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="9">
-        <v>452.0</v>
-      </c>
-      <c r="B37" s="9">
+      <c r="C35" s="6">
+        <v>0.72953752473741884</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="6">
+        <v>393</v>
+      </c>
+      <c r="B36" s="6">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.68516859239168293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="6">
+        <v>452</v>
+      </c>
+      <c r="B37" s="6">
         <v>7.5</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="6">
         <v>0.5618051263561058</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="9">
-        <v>520.0</v>
-      </c>
-      <c r="B38" s="9">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="6">
+        <v>520</v>
+      </c>
+      <c r="B38" s="6">
         <v>7.3</v>
       </c>
-      <c r="C38" s="9">
-        <v>0.5487449316394639</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="9">
-        <v>597.0</v>
-      </c>
-      <c r="B39" s="9">
+      <c r="C38" s="6">
+        <v>0.54874493163946392</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="6">
+        <v>597</v>
+      </c>
+      <c r="B39" s="6">
         <v>7.1</v>
       </c>
-      <c r="C39" s="9">
-        <v>0.5357322092239741</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="9">
-        <v>687.0</v>
-      </c>
-      <c r="B40" s="9">
+      <c r="C39" s="6">
+        <v>0.53573220922397413</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="6">
+        <v>687</v>
+      </c>
+      <c r="B40" s="6">
         <v>5.93</v>
       </c>
-      <c r="C40" s="9">
-        <v>0.4565172614480202</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="9">
-        <v>797.0</v>
-      </c>
-      <c r="B41" s="9">
+      <c r="C40" s="6">
+        <v>0.45651726144802018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="6">
+        <v>797</v>
+      </c>
+      <c r="B41" s="6">
         <v>5.48</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="6">
         <v>0.42373217956629167</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="9">
-        <v>957.0</v>
-      </c>
-      <c r="B42" s="9">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="6">
+        <v>957</v>
+      </c>
+      <c r="B42" s="6">
         <v>4.66</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="6">
         <v>0.3678402370595148</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="9">
-        <v>1148.0</v>
-      </c>
-      <c r="B43" s="9">
-        <v>4.52</v>
-      </c>
-      <c r="C43" s="9">
-        <v>0.3545545938216004</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="9">
-        <v>1378.0</v>
-      </c>
-      <c r="B44" s="9">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="6">
+        <v>1148</v>
+      </c>
+      <c r="B43" s="6">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="C43" s="6">
+        <v>0.35455459382160037</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="6">
+        <v>1378</v>
+      </c>
+      <c r="B44" s="6">
         <v>3.67</v>
       </c>
-      <c r="C44" s="9">
-        <v>0.2925706923121317</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="9">
-        <v>1540.0</v>
-      </c>
-      <c r="B45" s="9">
+      <c r="C44" s="6">
+        <v>0.29257069231213167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="6">
+        <v>1540</v>
+      </c>
+      <c r="B45" s="6">
         <v>3.59</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="6">
         <v>0.27848104064729434</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="9">
-        <v>1654.0</v>
-      </c>
-      <c r="B46" s="9">
+    <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="6">
+        <v>1654</v>
+      </c>
+      <c r="B46" s="6">
         <v>3.16</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="6">
         <v>0.25165341245451056</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="9">
-        <v>1800.0</v>
-      </c>
-      <c r="B47" s="9">
+    <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="6">
+        <v>1800</v>
+      </c>
+      <c r="B47" s="6">
         <v>3.04</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="6">
         <v>0.23954924337179612</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="9">
-        <v>2000.0</v>
-      </c>
-      <c r="B48" s="9">
+    <row r="48" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="6">
+        <v>2000</v>
+      </c>
+      <c r="B48" s="6">
         <v>2.87</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="6">
         <v>0.224412143165204</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>